<commit_message>
update for scheuling but sitll on development
</commit_message>
<xml_diff>
--- a/resources/scheduling.xlsx
+++ b/resources/scheduling.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="144">
   <si>
     <t>Name</t>
   </si>
@@ -39,24 +39,12 @@
     <t>Delay After Action(Sec)</t>
   </si>
   <si>
-    <t>/html/body/div/div/md-content/div/section/div[9]/button</t>
-  </si>
-  <si>
-    <t>/html/body/div/div/md-content/md-content/div[3]/md-content/md-list/div/div/div/div[1]/button</t>
-  </si>
-  <si>
-    <t>//*[@id="nameSeach"]</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
     <t>input</t>
   </si>
   <si>
-    <t>//a[@class="fc-day-grid-event fc-h-event fc-event fc-start fc-end fc-draggable"][1]</t>
-  </si>
-  <si>
     <t>/html/body/md-edit-dialog/div[2]/button[2]</t>
   </si>
   <si>
@@ -96,12 +84,6 @@
     <t>search input</t>
   </si>
   <si>
-    <t>select item</t>
-  </si>
-  <si>
-    <t>select first schedule on the calendar</t>
-  </si>
-  <si>
     <t>visit type</t>
   </si>
   <si>
@@ -120,21 +102,12 @@
     <t>Default Value</t>
   </si>
   <si>
-    <t>lastname</t>
-  </si>
-  <si>
     <t>//td[@ng-click="vm.updateVisitType($event)"]</t>
   </si>
   <si>
     <t>//form[@name="editDialog"]/md-input-container/md-select</t>
   </si>
   <si>
-    <t>/html/body/div/div/md-content/md-content/div[3]/md-content/md-list/md-list/md-list-item[1]/div/button</t>
-  </si>
-  <si>
-    <t>/html/body/div/div/md-content/div/section/div[7]/button</t>
-  </si>
-  <si>
     <t>Click Visit</t>
   </si>
   <si>
@@ -198,7 +171,283 @@
     <t>//md-option[@class="ng-scope md-ink-ripple"][1]</t>
   </si>
   <si>
-    <t>clinician_lastname</t>
+    <t>/html/body/div/div/md-content/div/section/div[10]/button</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/div/section/div[8]/button</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/md-content/div/md-content/md-list/div/div/div/div[1]/button</t>
+  </si>
+  <si>
+    <t>//input[@id="nameSeach"]</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/md-content/div/md-content/md-list/md-list/md-list-item[1]/div/button</t>
+  </si>
+  <si>
+    <t>(//md-card-header[@ng-click="vm.assignClinician(visitType.name, vm.episode.primaryClinicians[visitType.name])"])[1]</t>
+  </si>
+  <si>
+    <t>//md-dialog-content//button[@ng-click="vm.filterShow = !vm.filterShow"]</t>
+  </si>
+  <si>
+    <t>//md-dialog-content//input[@ng-model="vm.clinicianNameSearch"]</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/div/div[1]/div[1]/md-table-container/table/tbody/tr/td[1]/md-checkbox</t>
+  </si>
+  <si>
+    <t>select firt clinician result</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/div/div[1]/div[1]/md-input-container/div/button</t>
+  </si>
+  <si>
+    <t>click submit button</t>
+  </si>
+  <si>
+    <t>che</t>
+  </si>
+  <si>
+    <t>(//a[@class="fc-day-grid-event fc-h-event fc-event fc-start fc-end fc-draggable"])[1]</t>
+  </si>
+  <si>
+    <t>click first schedule</t>
+  </si>
+  <si>
+    <t>select first patient result</t>
+  </si>
+  <si>
+    <t>select assign clinician box</t>
+  </si>
+  <si>
+    <t>//div[@class="pg-loading-html pg-loaded"]</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>Update loading screen</t>
+  </si>
+  <si>
+    <t>checked</t>
+  </si>
+  <si>
+    <t>click assign visit type</t>
+  </si>
+  <si>
+    <t>//form[@name="editDialog"]//md-select</t>
+  </si>
+  <si>
+    <t>update visit type</t>
+  </si>
+  <si>
+    <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[1]</t>
+  </si>
+  <si>
+    <t>Click first visit type</t>
+  </si>
+  <si>
+    <t>//button[@aria-label="Save"]</t>
+  </si>
+  <si>
+    <t>save button click</t>
+  </si>
+  <si>
+    <t>//md-dialog//md-tab-item[3]</t>
+  </si>
+  <si>
+    <t>click Edit Task</t>
+  </si>
+  <si>
+    <t>input task</t>
+  </si>
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>//button[@ng-click="vm.addNewTask()"]</t>
+  </si>
+  <si>
+    <t>Add button Click</t>
+  </si>
+  <si>
+    <t>Task 2</t>
+  </si>
+  <si>
+    <t>(//button[@ng-click="vm.openEdit(task)"])[1]</t>
+  </si>
+  <si>
+    <t>(//textarea[@ng-model="vm.descriptionChange"])[1]</t>
+  </si>
+  <si>
+    <t>first description</t>
+  </si>
+  <si>
+    <t>input description</t>
+  </si>
+  <si>
+    <t>//md-dialog-content//div/div/div[1]/md-list/md-list-item[1]/div[1]/div[2]/button[2]</t>
+  </si>
+  <si>
+    <t>click checked</t>
+  </si>
+  <si>
+    <t>//md-dialog-content//div/div/div[1]/md-list/md-list-item[2]/div[1]/div[2]/button[4]</t>
+  </si>
+  <si>
+    <t>delete task</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/md-dialog/md-dialog-actions/button</t>
+  </si>
+  <si>
+    <t>close modal popup</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/md-content/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item[3]</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/form/md-card[1]/md-content/md-card[1]/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[1]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[1]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[2]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[2]</t>
+  </si>
+  <si>
+    <t>Visit</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>visit frequency</t>
+  </si>
+  <si>
+    <t>Add RN</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/form/md-card[1]/md-content/md-card[2]/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/form/md-card[1]/md-content/md-card[3]/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/form/md-card[1]/md-content/md-card[4]/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/form/md-card[1]/md-content/md-card[5]/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/form/md-card[1]/md-content/md-card[6]/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[3]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[3]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[4]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[4]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[6]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[6]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[7]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[7]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[8]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[8]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[9]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[9]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[10]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[10]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[11]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[11]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[12]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[12]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[13]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[13]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[14]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[14]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-thumb"])[5]</t>
+  </si>
+  <si>
+    <t>(//div[@class="_md-slider-wrapper"])[5]</t>
+  </si>
+  <si>
+    <t>//md-dialog-content/form/md-card[1]/md-content/md-card[7]/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item</t>
+  </si>
+  <si>
+    <t>//md-select[@ng-change="vm.orderTemplate(vm.value)"]</t>
+  </si>
+  <si>
+    <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[2]</t>
+  </si>
+  <si>
+    <t>/html/body/div[4]/md-dialog/md-dialog-actions/button[1]</t>
+  </si>
+  <si>
+    <t>gloria</t>
+  </si>
+  <si>
+    <t>//input[@ng-model="vm.charts.frequency.subject"]</t>
+  </si>
+  <si>
+    <t>//button[@aria-label="CSMAIL.COMPOSE_CSMAIL"]</t>
+  </si>
+  <si>
+    <t>button click</t>
   </si>
 </sst>
 </file>
@@ -539,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.28515625" defaultRowHeight="36.75" customHeight="1"/>
@@ -575,21 +824,21 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -603,13 +852,13 @@
     </row>
     <row r="3" spans="1:9" ht="36.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -623,13 +872,13 @@
     </row>
     <row r="4" spans="1:9" ht="36.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -643,13 +892,16 @@
     </row>
     <row r="5" spans="1:9" ht="36.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -658,21 +910,18 @@
         <v>1</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="36.75" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="50.25" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -684,15 +933,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="36.75" customHeight="1">
+    <row r="7" spans="1:9" ht="50.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -706,13 +955,13 @@
     </row>
     <row r="8" spans="1:9" ht="36.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -726,33 +975,30 @@
     </row>
     <row r="9" spans="1:9" ht="36.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="G9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="36.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -766,13 +1012,13 @@
     </row>
     <row r="11" spans="1:9" ht="36.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -786,13 +1032,13 @@
     </row>
     <row r="12" spans="1:9" ht="36.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -801,21 +1047,18 @@
         <v>1</v>
       </c>
       <c r="G12" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -827,16 +1070,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="36.75" customHeight="1">
+    <row r="14" spans="1:9" customFormat="1" ht="51" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="3">
         <v>1</v>
       </c>
@@ -849,16 +1093,13 @@
     </row>
     <row r="15" spans="1:9" ht="36.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -872,13 +1113,13 @@
     </row>
     <row r="16" spans="1:9" ht="36.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -892,13 +1133,13 @@
     </row>
     <row r="17" spans="1:8" ht="36.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -912,13 +1153,13 @@
     </row>
     <row r="18" spans="1:8" ht="36.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -932,27 +1173,36 @@
     </row>
     <row r="19" spans="1:8" ht="36.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="63" customHeight="1">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="36.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -966,13 +1216,16 @@
     </row>
     <row r="21" spans="1:8" ht="36.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -981,18 +1234,18 @@
         <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="36.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -1006,47 +1259,47 @@
     </row>
     <row r="23" spans="1:8" ht="36.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="36.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="3">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="36.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -1057,30 +1310,37 @@
       <c r="G25" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="36.75" customHeight="1">
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8" ht="63" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="36.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
@@ -1089,18 +1349,18 @@
         <v>1</v>
       </c>
       <c r="G27" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="36.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
@@ -1109,6 +1369,701 @@
         <v>1</v>
       </c>
       <c r="G28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="36.75" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="51" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="46.5" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="36.75" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="36.75" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="36.75" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="36.75" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B36" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B37" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B39" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B40" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B42" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B43" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B45" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B46" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B47" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B48" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B49" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B50" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <v>1</v>
+      </c>
+      <c r="G51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B52" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B53" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B54" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B55" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B56" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B57" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B58" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B59" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B60" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3">
+        <v>1</v>
+      </c>
+      <c r="G60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B61" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <v>1</v>
+      </c>
+      <c r="G61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B62" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B63" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B64" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B65" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="3">
+        <v>1</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B66" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="3">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1</v>
+      </c>
+      <c r="G66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B67" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="3">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="36.75" customHeight="1">
+      <c r="B68" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="3">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1</v>
+      </c>
+      <c r="G68" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1120,12 +2075,446 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="48.85546875" defaultRowHeight="51" customHeight="1"/>
+  <sheetData>
+    <row r="2" spans="1:7" ht="51" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="51" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="51" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="51" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="51" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="51" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="51" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="51" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="51" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="51" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="51" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="51" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="51" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="51" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="51" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="51" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="51" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="51" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="51" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix for scheduling clinician pt2
</commit_message>
<xml_diff>
--- a/resources/scheduling.xlsx
+++ b/resources/scheduling.xlsx
@@ -528,13 +528,13 @@
     <t>//td[@class="fc-event-container"]//span[contains(text(),'clinician ST1')]</t>
   </si>
   <si>
-    <t>//span[@ng-show="vm.episode.primaryClinicians[visitType.name].aggregateId" and contains(text(),"clinician Pt1")]</t>
-  </si>
-  <si>
     <t>pt2</t>
   </si>
   <si>
     <t>//td[@class="fc-event-container"]//span[contains(text(),'Clinician Pt2')]</t>
+  </si>
+  <si>
+    <t>//span[@ng-show="vm.episode.primaryClinicians[visitType.name].aggregateId" and contains(text(),"Clinician Pt2")]</t>
   </si>
 </sst>
 </file>
@@ -894,7 +894,7 @@
   <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150"/>
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.28515625" defaultRowHeight="36.75" customHeight="1"/>
@@ -1088,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G9" s="3">
         <v>3</v>
@@ -2638,7 +2638,7 @@
         <v>8</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G87" s="3">
         <v>3</v>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="150" spans="1:7" ht="36.75" customHeight="1">
       <c r="B150" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>34</v>
@@ -3873,7 +3873,7 @@
     </row>
     <row r="154" spans="1:7" ht="36.75" customHeight="1">
       <c r="B154" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
fix sched 3 to 4
</commit_message>
<xml_diff>
--- a/resources/scheduling.xlsx
+++ b/resources/scheduling.xlsx
@@ -493,9 +493,6 @@
     <t>//span[@ng-show="vm.episode.primaryClinicians[visitType.name].aggregateId" and contains(text(),"clinician pt3")]</t>
   </si>
   <si>
-    <t>pt3</t>
-  </si>
-  <si>
     <t>//button[@aria-label="Operations"]</t>
   </si>
   <si>
@@ -565,24 +562,6 @@
     <t>Preauth visit does not exist</t>
   </si>
   <si>
-    <t>msw3</t>
-  </si>
-  <si>
-    <t>ot3</t>
-  </si>
-  <si>
-    <t>rd3</t>
-  </si>
-  <si>
-    <t>st3</t>
-  </si>
-  <si>
-    <t>rn3</t>
-  </si>
-  <si>
-    <t>chha3</t>
-  </si>
-  <si>
     <t>//td[@class="fc-event-container"]//span[contains(text(),'clinician MSW3')]</t>
   </si>
   <si>
@@ -602,6 +581,27 @@
   </si>
   <si>
     <t>//td[@class="fc-event-container"]//span[contains(text(),'clinician Pt3')]</t>
+  </si>
+  <si>
+    <t>chha4</t>
+  </si>
+  <si>
+    <t>msw4</t>
+  </si>
+  <si>
+    <t>ot4</t>
+  </si>
+  <si>
+    <t>pt4</t>
+  </si>
+  <si>
+    <t>rd4</t>
+  </si>
+  <si>
+    <t>st4</t>
+  </si>
+  <si>
+    <t>rn4</t>
   </si>
 </sst>
 </file>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView tabSelected="1" topLeftCell="B133" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.28515625" defaultRowHeight="36.75" customHeight="1"/>
@@ -1000,7 +1000,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="36.75" customHeight="1">
@@ -1008,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="36.75" customHeight="1">
@@ -1031,7 +1031,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="36.75" customHeight="1">
@@ -1069,7 +1069,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
@@ -1096,7 +1096,7 @@
         <v>71</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="50.25" customHeight="1">
@@ -1119,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36.75" customHeight="1">
@@ -1142,7 +1142,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="36.75" customHeight="1">
@@ -1165,7 +1165,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:10" customFormat="1" ht="51" customHeight="1">
@@ -1189,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="36.75" customHeight="1">
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="36.75" customHeight="1">
@@ -1235,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="36.75" customHeight="1">
@@ -1258,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="36.75" customHeight="1">
@@ -1281,7 +1281,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="36.75" customHeight="1">
@@ -1307,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="36.75" customHeight="1">
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="36.75" customHeight="1">
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="36.75" customHeight="1">
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="36.75" customHeight="1">
@@ -1402,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="36.75" customHeight="1">
@@ -1419,7 +1419,7 @@
         <v>52</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="36.75" customHeight="1">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="H20"/>
       <c r="J20" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" customHeight="1">
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="36.75" customHeight="1">
@@ -1489,7 +1489,7 @@
         <v>3</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="36.75" customHeight="1">
@@ -1512,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="36.75" customHeight="1">
@@ -1526,13 +1526,13 @@
         <v>8</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G24" s="3">
         <v>3</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="36.75" customHeight="1">
@@ -1555,7 +1555,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="36.75" customHeight="1">
@@ -1578,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="36.75" customHeight="1">
@@ -1601,7 +1601,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="36.75" customHeight="1">
@@ -1624,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="36.75" customHeight="1">
@@ -1647,7 +1647,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="36.75" customHeight="1">
@@ -1670,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="36.75" customHeight="1">
@@ -1693,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="36.75" customHeight="1">
@@ -1716,7 +1716,7 @@
         <v>3</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="36.75" customHeight="1">
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="36.75" customHeight="1">
@@ -1765,7 +1765,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="36.75" customHeight="1">
@@ -1791,7 +1791,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="36.75" customHeight="1">
@@ -1814,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="36.75" customHeight="1">
@@ -1837,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="36.75" customHeight="1">
@@ -1854,7 +1854,7 @@
         <v>52</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="36.75" customHeight="1">
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="36.75" customHeight="1">
@@ -1900,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="36.75" customHeight="1">
@@ -1923,7 +1923,7 @@
         <v>3</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="36.75" customHeight="1">
@@ -1946,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="36.75" customHeight="1">
@@ -1960,13 +1960,13 @@
         <v>8</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="G43" s="3">
         <v>3</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="36.75" customHeight="1">
@@ -1989,7 +1989,7 @@
         <v>1</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="36.75" customHeight="1">
@@ -2012,7 +2012,7 @@
         <v>10</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="36.75" customHeight="1">
@@ -2035,7 +2035,7 @@
         <v>3</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="36.75" customHeight="1">
@@ -2058,7 +2058,7 @@
         <v>2</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="36.75" customHeight="1">
@@ -2081,7 +2081,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="36.75" customHeight="1">
@@ -2104,7 +2104,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="36.75" customHeight="1">
@@ -2127,7 +2127,7 @@
         <v>3</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="36.75" customHeight="1">
@@ -2150,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="36.75" customHeight="1">
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="36.75" customHeight="1">
@@ -2199,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="36.75" customHeight="1">
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="36.75" customHeight="1">
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="36.75" customHeight="1">
@@ -2271,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="36.75" customHeight="1">
@@ -2288,7 +2288,7 @@
         <v>52</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="36.75" customHeight="1">
@@ -2311,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="36.75" customHeight="1">
@@ -2334,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="36.75" customHeight="1">
@@ -2357,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="36.75" customHeight="1">
@@ -2380,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="36.75" customHeight="1">
@@ -2394,13 +2394,13 @@
         <v>8</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G62" s="3">
         <v>3</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="36.75" customHeight="1">
@@ -2423,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="36.75" customHeight="1">
@@ -2446,7 +2446,7 @@
         <v>10</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="36.75" customHeight="1">
@@ -2469,7 +2469,7 @@
         <v>3</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="36.75" customHeight="1">
@@ -2492,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="36.75" customHeight="1">
@@ -2515,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="36.75" customHeight="1">
@@ -2538,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="36.75" customHeight="1">
@@ -2561,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="36.75" customHeight="1">
@@ -2584,7 +2584,7 @@
         <v>3</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="36.75" customHeight="1">
@@ -2610,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="36.75" customHeight="1">
@@ -2633,7 +2633,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="36.75" customHeight="1">
@@ -2659,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="36.75" customHeight="1">
@@ -2682,7 +2682,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="36.75" customHeight="1">
@@ -2705,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="36.75" customHeight="1">
@@ -2722,7 +2722,7 @@
         <v>52</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="36.75" customHeight="1">
@@ -2745,7 +2745,7 @@
         <v>1</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="36.75" customHeight="1">
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="36.75" customHeight="1">
@@ -2791,7 +2791,7 @@
         <v>3</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="36.75" customHeight="1">
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="36.75" customHeight="1">
@@ -2828,13 +2828,13 @@
         <v>8</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>157</v>
+        <v>190</v>
       </c>
       <c r="G81" s="3">
         <v>3</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="36.75" customHeight="1">
@@ -2857,7 +2857,7 @@
         <v>1</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="36.75" customHeight="1">
@@ -2880,7 +2880,7 @@
         <v>10</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="36.75" customHeight="1">
@@ -2903,7 +2903,7 @@
         <v>3</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="36.75" customHeight="1">
@@ -2926,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="36.75" customHeight="1">
@@ -2949,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="36.75" customHeight="1">
@@ -2972,7 +2972,7 @@
         <v>1</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="36.75" customHeight="1">
@@ -2995,7 +2995,7 @@
         <v>1</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="36.75" customHeight="1">
@@ -3018,7 +3018,7 @@
         <v>3</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="36.75" customHeight="1">
@@ -3044,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="36.75" customHeight="1">
@@ -3067,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="36.75" customHeight="1">
@@ -3093,7 +3093,7 @@
         <v>1</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="36.75" customHeight="1">
@@ -3116,7 +3116,7 @@
         <v>1</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="36.75" customHeight="1">
@@ -3139,7 +3139,7 @@
         <v>1</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="36.75" customHeight="1">
@@ -3156,7 +3156,7 @@
         <v>52</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="36.75" customHeight="1">
@@ -3179,7 +3179,7 @@
         <v>1</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="36.75" customHeight="1">
@@ -3202,7 +3202,7 @@
         <v>1</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="36.75" customHeight="1">
@@ -3225,7 +3225,7 @@
         <v>1</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="36.75" customHeight="1">
@@ -3248,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="36.75" customHeight="1">
@@ -3262,13 +3262,13 @@
         <v>8</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="G100" s="3">
         <v>3</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="36.75" customHeight="1">
@@ -3291,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="36.75" customHeight="1">
@@ -3314,7 +3314,7 @@
         <v>10</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="36.75" customHeight="1">
@@ -3337,7 +3337,7 @@
         <v>1</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="36.75" customHeight="1">
@@ -3360,7 +3360,7 @@
         <v>1</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="36.75" customHeight="1">
@@ -3383,7 +3383,7 @@
         <v>1</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="36.75" customHeight="1">
@@ -3406,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="36.75" customHeight="1">
@@ -3429,7 +3429,7 @@
         <v>1</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="36.75" customHeight="1">
@@ -3452,7 +3452,7 @@
         <v>3</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="36.75" customHeight="1">
@@ -3478,7 +3478,7 @@
         <v>1</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="36.75" customHeight="1">
@@ -3501,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="36.75" customHeight="1">
@@ -3527,7 +3527,7 @@
         <v>1</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="36.75" customHeight="1">
@@ -3550,7 +3550,7 @@
         <v>1</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="36.75" customHeight="1">
@@ -3573,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="36.75" customHeight="1">
@@ -3590,7 +3590,7 @@
         <v>52</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="36.75" customHeight="1">
@@ -3613,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="J115" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="36.75" customHeight="1">
@@ -3636,7 +3636,7 @@
         <v>1</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="36.75" customHeight="1">
@@ -3659,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="J117" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="36.75" customHeight="1">
@@ -3682,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="J118" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="36.75" customHeight="1">
@@ -3696,13 +3696,13 @@
         <v>8</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="G119" s="3">
         <v>3</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="36.75" customHeight="1">
@@ -3725,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="J120" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="36.75" customHeight="1">
@@ -3748,7 +3748,7 @@
         <v>10</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="36.75" customHeight="1">
@@ -3771,7 +3771,7 @@
         <v>3</v>
       </c>
       <c r="J122" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="36.75" customHeight="1">
@@ -3794,7 +3794,7 @@
         <v>1</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="36.75" customHeight="1">
@@ -3817,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="J124" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="125" spans="1:10" ht="36.75" customHeight="1">
@@ -3840,7 +3840,7 @@
         <v>1</v>
       </c>
       <c r="J125" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="126" spans="1:10" ht="36.75" customHeight="1">
@@ -3863,7 +3863,7 @@
         <v>2</v>
       </c>
       <c r="J126" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="127" spans="1:10" ht="36.75" customHeight="1">
@@ -3886,7 +3886,7 @@
         <v>3</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="128" spans="1:10" ht="36.75" customHeight="1">
@@ -3912,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="J128" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="129" spans="1:10" ht="36.75" customHeight="1">
@@ -3935,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="J129" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="36.75" customHeight="1">
@@ -3961,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="J130" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:10" ht="36.75" customHeight="1">
@@ -3984,7 +3984,7 @@
         <v>1</v>
       </c>
       <c r="J131" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="132" spans="1:10" ht="36.75" customHeight="1">
@@ -4007,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="133" spans="1:10" ht="36.75" customHeight="1">
@@ -4024,7 +4024,7 @@
         <v>52</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="134" spans="1:10" ht="36.75" customHeight="1">
@@ -4047,7 +4047,7 @@
         <v>1</v>
       </c>
       <c r="J134" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="36.75" customHeight="1">
@@ -4070,7 +4070,7 @@
         <v>1</v>
       </c>
       <c r="J135" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="36.75" customHeight="1">
@@ -4093,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="J136" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="137" spans="1:10" ht="36.75" customHeight="1">
@@ -4116,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="J137" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="138" spans="1:10" ht="36.75" customHeight="1">
@@ -4130,13 +4130,13 @@
         <v>8</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="G138" s="3">
         <v>3</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="139" spans="1:10" ht="36.75" customHeight="1">
@@ -4159,7 +4159,7 @@
         <v>1</v>
       </c>
       <c r="J139" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="140" spans="1:10" ht="36.75" customHeight="1">
@@ -4182,84 +4182,84 @@
         <v>10</v>
       </c>
       <c r="J140" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="141" spans="1:10" ht="36.75" customHeight="1">
       <c r="B141" s="3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J141" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="142" spans="1:10" ht="36.75" customHeight="1">
       <c r="B142" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J142" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="143" spans="1:10" ht="36.75" customHeight="1">
       <c r="B143" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="144" spans="1:10" ht="36.75" customHeight="1">
       <c r="B144" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J144" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="145" spans="2:10" ht="36.75" customHeight="1">
       <c r="B145" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J145" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="146" spans="2:10" ht="36.75" customHeight="1">
       <c r="B146" s="3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J146" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="147" spans="2:10" ht="36.75" customHeight="1">
       <c r="B147" s="3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J147" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -4272,7 +4272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J4" sqref="J4:J6"/>
     </sheetView>
   </sheetViews>
@@ -4314,7 +4314,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1">
@@ -4322,7 +4322,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -4337,7 +4337,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1">
@@ -4345,7 +4345,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -4360,7 +4360,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17.25" customHeight="1">
@@ -4383,7 +4383,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1">
@@ -4410,7 +4410,7 @@
         <v>71</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17.25" customHeight="1">
@@ -4433,7 +4433,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="17.25" customHeight="1">
@@ -4456,7 +4456,7 @@
         <v>3</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17.25" customHeight="1">
@@ -4467,7 +4467,7 @@
         <v>60</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17.25" customHeight="1">
@@ -4490,7 +4490,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17.25" customHeight="1">
@@ -4513,7 +4513,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17.25" customHeight="1">
@@ -4536,7 +4536,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="17.25" customHeight="1">
@@ -4559,7 +4559,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17.25" customHeight="1">
@@ -4582,7 +4582,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17.25" customHeight="1">
@@ -4605,7 +4605,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17.25" customHeight="1">
@@ -4625,7 +4625,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="17.25" customHeight="1">
@@ -4645,7 +4645,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="17.25" customHeight="1">
@@ -4665,7 +4665,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="17.25" customHeight="1">
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="17.25" customHeight="1">
@@ -4705,7 +4705,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="17.25" customHeight="1">
@@ -4725,7 +4725,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="17.25" customHeight="1">
@@ -4745,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="17.25" customHeight="1">
@@ -4765,7 +4765,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="17.25" customHeight="1">
@@ -4785,7 +4785,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="17.25" customHeight="1">
@@ -4805,7 +4805,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="17.25" customHeight="1">
@@ -4825,7 +4825,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="17.25" customHeight="1">
@@ -4845,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="17.25" customHeight="1">
@@ -4865,7 +4865,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="17.25" customHeight="1">
@@ -4885,7 +4885,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="17.25" customHeight="1">
@@ -4905,7 +4905,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="17.25" customHeight="1">
@@ -4925,7 +4925,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="17.25" customHeight="1">
@@ -4945,7 +4945,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="17.25" customHeight="1">
@@ -4965,7 +4965,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="17.25" customHeight="1">
@@ -4985,7 +4985,7 @@
         <v>1</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="17.25" customHeight="1">
@@ -5005,7 +5005,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="17.25" customHeight="1">
@@ -5025,7 +5025,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17.25" customHeight="1">
@@ -5045,7 +5045,7 @@
         <v>1</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17.25" customHeight="1">
@@ -5065,7 +5065,7 @@
         <v>1</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="17.25" customHeight="1">
@@ -5085,7 +5085,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="17.25" customHeight="1">
@@ -5105,7 +5105,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="17.25" customHeight="1">
@@ -5125,7 +5125,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="17.25" customHeight="1">
@@ -5145,7 +5145,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="17.25" customHeight="1">
@@ -5165,7 +5165,7 @@
         <v>1</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="17.25" customHeight="1">
@@ -5185,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="17.25" customHeight="1">
@@ -5205,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="17.25" customHeight="1">
@@ -5225,7 +5225,7 @@
         <v>1</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="17.25" customHeight="1">
@@ -5245,7 +5245,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="17.25" customHeight="1">
@@ -5265,7 +5265,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="17.25" customHeight="1">
@@ -5288,7 +5288,7 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="17.25" customHeight="1">
@@ -5302,7 +5302,7 @@
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
       <c r="J49" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -5353,7 +5353,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30">
@@ -5361,7 +5361,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -5376,7 +5376,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30">
@@ -5384,7 +5384,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -5399,7 +5399,7 @@
         <v>5</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60">
@@ -5410,7 +5410,7 @@
         <v>110</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60">
@@ -5430,7 +5430,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45">
@@ -5450,7 +5450,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60">
@@ -5461,7 +5461,7 @@
         <v>110</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60">
@@ -5481,7 +5481,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45">
@@ -5501,7 +5501,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60">
@@ -5512,7 +5512,7 @@
         <v>110</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60">
@@ -5532,7 +5532,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45">
@@ -5552,7 +5552,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60">
@@ -5563,7 +5563,7 @@
         <v>110</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60">
@@ -5583,7 +5583,7 @@
         <v>5</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45">
@@ -5603,7 +5603,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="60">
@@ -5614,7 +5614,7 @@
         <v>110</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="60">
@@ -5634,7 +5634,7 @@
         <v>5</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="45">
@@ -5654,7 +5654,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="60">
@@ -5665,7 +5665,7 @@
         <v>110</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="60">
@@ -5685,7 +5685,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="45">
@@ -5705,7 +5705,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="60">
@@ -5716,7 +5716,7 @@
         <v>110</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="60">
@@ -5736,7 +5736,7 @@
         <v>5</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="45">
@@ -5756,7 +5756,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="60">
@@ -5767,7 +5767,7 @@
         <v>110</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="60">
@@ -5787,7 +5787,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="45">
@@ -5807,7 +5807,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="60">
@@ -5818,7 +5818,7 @@
         <v>110</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="60">
@@ -5838,7 +5838,7 @@
         <v>5</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -5896,7 +5896,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -5904,7 +5904,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -5919,7 +5919,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5927,7 +5927,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -5942,7 +5942,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45">
@@ -5965,7 +5965,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -5992,7 +5992,7 @@
         <v>71</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60">
@@ -6012,7 +6012,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30">
@@ -6035,7 +6035,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60">
@@ -6058,7 +6058,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30">
@@ -6078,7 +6078,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30">
@@ -6098,7 +6098,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60">
@@ -6118,7 +6118,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30">
@@ -6138,7 +6138,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -6191,7 +6191,7 @@
         <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30">
@@ -6199,7 +6199,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -6214,7 +6214,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30">
@@ -6222,7 +6222,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -6237,7 +6237,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60">
@@ -6260,7 +6260,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6287,7 +6287,7 @@
         <v>71</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60">
@@ -6310,7 +6310,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60">
@@ -6321,7 +6321,7 @@
         <v>33</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60">
@@ -6332,7 +6332,7 @@
         <v>33</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60">
@@ -6343,7 +6343,7 @@
         <v>33</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60">
@@ -6354,7 +6354,7 @@
         <v>33</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60">
@@ -6365,7 +6365,7 @@
         <v>33</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="60">
@@ -6376,7 +6376,7 @@
         <v>33</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60">
@@ -6387,7 +6387,7 @@
         <v>33</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create new comm notes test cases
</commit_message>
<xml_diff>
--- a/resources/scheduling.xlsx
+++ b/resources/scheduling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" activeTab="7"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="backup" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
     <sheet name="AddSched" sheetId="8" r:id="rId8"/>
+    <sheet name="CommNotes" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="231">
   <si>
     <t>Name</t>
   </si>
@@ -654,6 +655,66 @@
   </si>
   <si>
     <t>//button[@ng-click="vm.filterShow = false; vm.focusInput()"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-admin-email"]/md-content/md-card/md-card-content/md-content/md-tabs/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item[4]</t>
+  </si>
+  <si>
+    <t>//button[@ng-click="vmt.composeClick(null, 'ADD')"]</t>
+  </si>
+  <si>
+    <t>(//form[@name="emailForm"]//input)[1]</t>
+  </si>
+  <si>
+    <t>Case Conference Note</t>
+  </si>
+  <si>
+    <t>//md-virtual-repeat-container[@class="md-autocomplete-suggestions-container md-whiteframe-z1 md-virtual-repeat-container md-orient-vertical md-cs-content-theme-theme"]//li[1]</t>
+  </si>
+  <si>
+    <t>(//form[@name="emailForm"]//input)[4]</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>//md-virtual-repeat-container[@class="md-autocomplete-suggestions-container md-whiteframe-z1 md-virtual-repeat-container md-orient-vertical md-cs-content-theme-theme"]//li[2]</t>
+  </si>
+  <si>
+    <t>(//form[@name="emailForm"]//md-select)</t>
+  </si>
+  <si>
+    <t>//button[@translate="ADD"]</t>
+  </si>
+  <si>
+    <t>//p[contains(text(),"CASE CONFERENCE NOTE")]</t>
+  </si>
+  <si>
+    <t>faile to create comm notest</t>
+  </si>
+  <si>
+    <t>Comm Notes</t>
+  </si>
+  <si>
+    <t>Add button</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>author name</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>verify comm notes</t>
   </si>
 </sst>
 </file>
@@ -8754,8 +8815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="18" customHeight="1"/>
@@ -9222,4 +9283,419 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="78.5703125" style="3" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="3"/>
+    <col min="10" max="10" width="42.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="B5" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30">
+      <c r="A9" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45">
+      <c r="A11" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45">
+      <c r="A12" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45">
+      <c r="A14" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30">
+      <c r="A16" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix add and delete scheduling
</commit_message>
<xml_diff>
--- a/resources/scheduling.xlsx
+++ b/resources/scheduling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" activeTab="7"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -720,7 +720,7 @@
     <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[4]</t>
   </si>
   <si>
-    <t>(//div[@id="fullCalendar"]//span[conD:\SE\Documents\Desktop\test.pngtains(text(),"MSW")]/../../../a[@class="fc-day-grid-event fc-h-event fc-event fc-start fc-end fc-draggable"])[1]</t>
+    <t>(//div[@id="fullCalendar"]//span[contains(text(),"MSW")])[2]/../../../a[@class="fc-day-grid-event fc-h-event fc-event fc-start fc-end fc-draggable"]</t>
   </si>
 </sst>
 </file>
@@ -8821,8 +8821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="18" customHeight="1"/>

</xml_diff>

<commit_message>
update for scheduling and all
</commit_message>
<xml_diff>
--- a/resources/scheduling.xlsx
+++ b/resources/scheduling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" activeTab="8"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -618,9 +618,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>//*[@id="compliance-tabs"]/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item[2]</t>
-  </si>
-  <si>
     <t>//button[@aria-label="Administration" and @ng-click="vm.go(entry.state)"]</t>
   </si>
   <si>
@@ -715,6 +712,9 @@
   </si>
   <si>
     <t>(//button[@aria-label="CSMAIL.COMPOSE_CSMAIL"])[3]</t>
+  </si>
+  <si>
+    <t>//*[@id="compliance-tabs"]/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item[3]</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1162,7 @@
         <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="3" spans="1:10" ht="36.75" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -1205,7 +1205,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -1248,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -1287,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>151</v>
@@ -1298,7 +1298,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -4019,7 +4019,7 @@
         <v>37</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>7</v>
@@ -4471,7 +4471,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="17.25" customHeight="1"/>
@@ -4520,7 +4520,7 @@
         <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -4540,7 +4540,7 @@
     </row>
     <row r="3" spans="1:10" ht="36.75" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -4563,7 +4563,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4606,7 +4606,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -4645,7 +4645,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>151</v>
@@ -4656,7 +4656,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -4679,7 +4679,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -4699,7 +4699,7 @@
     </row>
     <row r="10" spans="1:10" ht="17.25" customHeight="1">
       <c r="B10" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>57</v>
@@ -4713,7 +4713,7 @@
         <v>68</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
@@ -4788,7 +4788,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -5557,7 +5557,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15"/>
@@ -5604,7 +5604,7 @@
         <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -5624,7 +5624,7 @@
     </row>
     <row r="3" spans="1:10" ht="36.75" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -5647,7 +5647,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -5667,7 +5667,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -6133,8 +6133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.42578125" defaultRowHeight="15"/>
@@ -6187,7 +6187,7 @@
         <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -6207,7 +6207,7 @@
     </row>
     <row r="3" spans="1:10" ht="36.75" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -6230,7 +6230,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -6250,7 +6250,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -6273,7 +6273,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -6312,7 +6312,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>151</v>
@@ -6320,7 +6320,7 @@
     </row>
     <row r="8" spans="1:10" ht="45">
       <c r="B8" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -6480,7 +6480,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15"/>
@@ -6528,7 +6528,7 @@
         <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -6548,7 +6548,7 @@
     </row>
     <row r="3" spans="1:10" ht="36.75" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -6571,7 +6571,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -6591,7 +6591,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -6614,7 +6614,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -6653,7 +6653,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>151</v>
@@ -6664,7 +6664,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -8827,7 +8827,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="18" customHeight="1"/>
@@ -8876,7 +8876,7 @@
         <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -8896,7 +8896,7 @@
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -8919,7 +8919,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -8939,7 +8939,7 @@
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -8962,7 +8962,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -9001,7 +9001,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>151</v>
@@ -9012,7 +9012,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -9134,13 +9134,13 @@
     </row>
     <row r="15" spans="1:10" ht="19.5" customHeight="1">
       <c r="B15" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
@@ -9154,7 +9154,7 @@
     </row>
     <row r="16" spans="1:10" ht="50.25" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -9276,7 +9276,7 @@
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1">
       <c r="B23" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>7</v>
@@ -9310,10 +9310,10 @@
     </row>
     <row r="25" spans="2:8" ht="18" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -9338,8 +9338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9387,7 +9387,7 @@
         <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -9407,7 +9407,7 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
@@ -9430,7 +9430,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
@@ -9450,7 +9450,7 @@
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -9473,7 +9473,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -9512,7 +9512,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>151</v>
@@ -9523,7 +9523,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -9543,10 +9543,10 @@
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="28.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -9563,15 +9563,15 @@
       <c r="H9"/>
       <c r="I9"/>
       <c r="J9" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>57</v>
@@ -9583,15 +9583,15 @@
         <v>3</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
@@ -9606,35 +9606,35 @@
         <v>5</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45">
       <c r="A12" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G12" s="3">
         <v>3</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45">
       <c r="A13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
@@ -9646,15 +9646,15 @@
         <v>3</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
@@ -9666,12 +9666,12 @@
         <v>3</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30">
       <c r="A15" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>36</v>
@@ -9686,15 +9686,15 @@
         <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -9706,13 +9706,13 @@
         <v>10</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>57</v>
@@ -9721,15 +9721,15 @@
         <v>3</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>30</v>
@@ -9738,7 +9738,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set patient to active
</commit_message>
<xml_diff>
--- a/resources/scheduling.xlsx
+++ b/resources/scheduling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" activeTab="8"/>
+    <workbookView xWindow="14505" yWindow="-15" windowWidth="14340" windowHeight="13380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
     <sheet name="AddSched" sheetId="8" r:id="rId8"/>
     <sheet name="CommNotes" sheetId="9" r:id="rId9"/>
+    <sheet name="SetActive" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="235">
   <si>
     <t>Name</t>
   </si>
@@ -715,6 +716,18 @@
   </si>
   <si>
     <t>//*[@id="compliance-tabs"]/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item[2]</t>
+  </si>
+  <si>
+    <t>//md-card//button[@ng-click="$mdOpenMenu($event)"]</t>
+  </si>
+  <si>
+    <t>//div[@class="_md _md-open-menu-container md-whiteframe-z2 md-cs-content-theme-theme _md-active _md-clickable"]//md-menu-item[2]</t>
+  </si>
+  <si>
+    <t>//md-dialog//button[@aria-label="Confirm"]</t>
+  </si>
+  <si>
+    <t>//*[@id="compliance-tabs"]/md-tabs-wrapper/md-tabs-canvas/md-pagination-wrapper/md-tab-item[3]</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.28515625" defaultRowHeight="36.75" customHeight="1"/>
@@ -1214,7 +1227,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -4457,6 +4470,398 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="33" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="95.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="33" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="33" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="33" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="33" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="33" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="33" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="33" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="33" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="33" customHeight="1">
+      <c r="B9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="33" customHeight="1">
+      <c r="B10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="33" customHeight="1">
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="33" customHeight="1">
+      <c r="B12" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="33" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="33" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="33" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4577,7 +4982,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -6127,8 +6532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.42578125" defaultRowHeight="15"/>
@@ -6244,7 +6649,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -6303,7 +6708,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>212</v>
@@ -6326,7 +6731,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>151</v>
@@ -6473,8 +6878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15"/>
@@ -6585,7 +6990,7 @@
     </row>
     <row r="5" spans="1:10" ht="36.75" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -8821,7 +9226,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="18" customHeight="1"/>
@@ -8933,7 +9338,7 @@
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
@@ -9332,8 +9737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9444,7 +9849,7 @@
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>

</xml_diff>